<commit_message>
Framework changes and add TC01 for phs000463
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000463_Diagnosis-ActeLymphoblsLeukNOS_Sex-Male.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000463_Diagnosis-ActeLymphoblsLeukNOS_Sex-Male.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5E09BA-AA59-4882-BE49-4FA615041210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4062E59-0598-0348-B9DE-F9855A3E59FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="1815" windowWidth="22275" windowHeight="12480" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="13680" yWindow="-24620" windowWidth="35000" windowHeight="25180" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,246 +71,289 @@
     <t>TC01_CCDI_phs000463_Diagnosis-ClrearCellSacrKidn_Sex-Male_WebData.xlsx</t>
   </si>
   <si>
-    <t>with file_data as (
-select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
-SELECT fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type" ,
-        CASE     
-    WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        END
-    WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        END
-    WHEN fd.file_size &gt;= 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-            ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-        END
-    ELSE 
-        CASE 
-            WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-            ELSE ROUND(fd.file_size, 2) || ' Bytes'
-        END
-END AS "File Size",
-fd.file_access AS "File Access", std.dbgap_accession AS "Study ID", fd.participantid AS "Participant ID", null as "Sample ID"
-FROM 
-    df_study std
- LEFT JOIN  
-    file_data fd ON std.id = fd.studyid
+    <t>WITH diagnosis_summary AS (  
+  SELECT 
+    d."participant.id"                                AS participant_id, 
+    GROUP_CONCAT(DISTINCT d.age_at_diagnosis)         AS age_at_diagnosis, 
+    GROUP_CONCAT(DISTINCT d.diagnosis)                AS diagnosis, 
+    GROUP_CONCAT(DISTINCT d.anatomic_site)            AS anatomic_site,
+    GROUP_CONCAT(DISTINCT d.diagnosis_category)       AS diagnosis_category
+  FROM df_diagnosis d
+  WHERE d."participant.id" IS NOT NULL
+  GROUP BY d."participant.id"
+),
+survival_summary AS (
+  SELECT 
+    s."participant.id"                                AS participant_id,
+    GROUP_CONCAT(DISTINCT s.last_known_survival_status) AS last_known_survival_status
+  FROM df_survival s
+  GROUP BY s."participant.id"
+)
+SELECT
+  prt.participant_id                           AS "Participant ID",
+  std.dbgap_accession                          AS "Study ID",
+  COALESCE(prt.sex_at_birth, '')               AS "Sex",
+  COALESCE(prt.race, '')                       AS "Race",
+  COALESCE(dsum.diagnosis, '')                 AS "Diagnosis",
+  COALESCE(dsum.anatomic_site, '')             AS "Diagnosis Anatomic Site",
+  COALESCE(dsum.diagnosis_category, '')        AS "Diagnosis_Category",
+  COALESCE(
+    CASE WHEN dsum.age_at_diagnosis = '-999' THEN 'Not Reported' ELSE dsum.age_at_diagnosis END,
+    ''
+  )                                            AS "Age at Diagnosis (days)",
+  NULL                                         AS "Treatment Type",
+  COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
+FROM df_study std
+LEFT JOIN df_consent_group  cg   ON std.id = cg."study.id"
+LEFT JOIN df_participant    prt  ON cg.id  = prt."consent_group.id"
+LEFT JOIN diagnosis_summary dsum ON prt.id = dsum.participant_id
+LEFT JOIN survival_summary  srv  ON prt.id = srv.participant_id
 WHERE 
-    std.dbgap_accession = 'phs000463'</t>
+  std.dbgap_accession = 'phs000463'
+  AND prt.sex_at_birth = 'Male'
+  AND EXISTS (
+    SELECT 1
+    FROM df_diagnosis d
+    WHERE d."participant.id" = prt.id
+      AND d.diagnosis = 'Acute Lymphoblastic Leukemia, NOS'
+  )
+ORDER BY prt.participant_id ASC
+LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT
-    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT prt.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT cmf.id)) AS "Files"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-Left JOIN 
-    df_diagnosis diag ON prt.id = diag."participant.id"     
-LEFT JOIN 
-    df_clinical_measure_file cmf ON std.id = cmf."study.id"
+  COUNT(DISTINCT std.dbgap_accession) AS "Studies",
+  COUNT(DISTINCT prt.participant_id)  AS "Participants",
+  CAST(0 AS INTEGER)                  AS "Samples",  -- no df_sample in this dataset
+  COUNT(DISTINCT cmf.id)              AS "Files"     -- clinical files tied to study
+FROM df_study std
+LEFT JOIN df_consent_group  cg  ON std.id = cg."study.id"
+LEFT JOIN df_participant    prt ON cg.id  = prt."consent_group.id"
+LEFT JOIN df_clinical_measure_file cmf ON std.id = cmf."study.id"   -- &lt;-- changed here
 WHERE 
-    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Male' and diag.diagnosis = 'Acute Lymphoblastic Leukemia, NOS' ;</t>
-  </si>
-  <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ) 
+  std.dbgap_accession = 'phs000463'
+  AND prt.sex_at_birth = 'Male'
+  AND EXISTS (
+    SELECT 1
+    FROM df_diagnosis d
+    WHERE d."participant.id" = prt.id
+      AND d.diagnosis = 'Acute Lymphoblastic Leukemia, NOS'
+  );</t>
+  </si>
+  <si>
+    <t>WITH Study AS (
+  SELECT std.id AS study_row_id, std.dbgap_accession AS study_id,
+         std.study_name AS study_name, std.study_status AS study_status
+  FROM df_study std
+  WHERE std.dbgap_accession = 'phs000463'
+  LIMIT 1
+),
+-- all participants for the study (no filters)
+AllStudyParticipants AS (
+  SELECT prt.id AS participant_id
+  FROM df_participant prt
+  JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  JOIN Study s ON cg."study.id" = s.study_row_id
+),
+DiagTop AS (
+  SELECT d.diagnosis, COUNT(*) AS cnt
+  FROM df_diagnosis d
+  JOIN AllStudyParticipants ap ON ap.participant_id = d."participant.id"
+  GROUP BY d.diagnosis
+  ORDER BY cnt DESC, d.diagnosis
+  LIMIT 5
+),
+DiagAgg AS (
+  SELECT (SELECT study_id FROM Study) AS study_id,
+         GROUP_CONCAT(d.diagnosis || ' (' || d.cnt || ')', CHAR(10)) AS diagcount
+  FROM DiagTop d
+),
+AnatTop AS (
+  SELECT d.anatomic_site AS anat, COUNT(*) AS cnt
+  FROM df_diagnosis d
+  JOIN AllStudyParticipants ap ON ap.participant_id = d."participant.id"
+  GROUP BY d.anatomic_site
+  ORDER BY cnt DESC, anat
+  LIMIT 5
+),
+AnatAgg AS (
+  SELECT (SELECT study_id FROM Study) AS study_id,
+         GROUP_CONCAT(a.anat || ' (' || a.cnt || ')', CHAR(10)) AS anatcount
+  FROM AnatTop a
+),
+Participants AS (
+  SELECT (SELECT study_id FROM Study) AS study_id,
+         COUNT(*) AS p_count
+  FROM AllStudyParticipants
+),
+-- samples fixed at 0 for this dataset
+Samples AS (
+  SELECT (SELECT study_id FROM Study) AS study_id, 0 AS s_count
+),
+TotalFiles AS (
+  SELECT s.study_id, COUNT(DISTINCT cmf.id) AS file_count
+  FROM df_clinical_measure_file cmf
+  JOIN Study s ON cmf."study.id" = s.study_row_id
+),
+FileTop AS (
+  SELECT cmf.file_type, COUNT(*) AS cnt
+  FROM df_clinical_measure_file cmf
+  JOIN Study s ON cmf."study.id" = s.study_row_id
+  GROUP BY cmf.file_type
+  ORDER BY cnt DESC, cmf.file_type
+  LIMIT 5
+),
+FileAgg AS (
+  SELECT (SELECT study_id FROM Study) AS study_id,
+         GROUP_CONCAT(file_type || ' (' || cnt || ')', CHAR(10)) AS file
+  FROM FileTop
+),
+-- publications / personnel / funding (unchanged except DISTINCT fix you already made)
+Publications AS (
+  SELECT s.study_id,
+         (SELECT GROUP_CONCAT(pubmed_id, ';')
+            FROM (SELECT p.pubmed_id
+                  FROM df_publication p
+                  WHERE p."study.id" = s.study_row_id
+                  ORDER BY CAST(p.pubmed_id AS INTEGER) ASC) ord) AS pubmeds
+  FROM Study s
+),
+Personnel AS (
+  SELECT s.study_id, GROUP_CONCAT(personnel_name, ';') AS name
+  FROM df_study_personnel sp
+  JOIN Study s ON sp."study.id" = s.study_row_id
+),
+Funding AS (
+  SELECT s.study_id,
+         GROUP_CONCAT(f.grant_id, ';') AS grant
+  FROM (SELECT DISTINCT grant_id, "study.id" FROM df_study_funding) f
+  JOIN Study s ON f."study.id" = s.study_row_id
+)
+SELECT
+  s.study_name    AS "Study Name",
+  s.study_id      AS "Study ID",
+  s.study_status  AS "Study Status",
+  d.diagcount     AS "Diagnosis (Top 5)",
+  a.anatcount     AS "Diagnosis Anatomic Site (Top 5)",
+  p.p_count       AS "Number of Participants",
+  sm.s_count      AS "Number of Samples",
+  tf.file_count   AS "Number of Files",
+  fa.file         AS "File Type (Top 5)",
+  pub.pubmeds     AS "PubMed ID",
+  pr.name         AS "Principal Investigator(s)",
+  fd.grant        AS "Grant ID"
+FROM Study s
+LEFT JOIN DiagAgg       d  ON s.study_id = d.study_id
+LEFT JOIN AnatAgg       a  ON s.study_id = a.study_id
+LEFT JOIN Participants  p  ON s.study_id = p.study_id
+LEFT JOIN Samples       sm ON s.study_id = sm.study_id
+LEFT JOIN TotalFiles    tf ON s.study_id = tf.study_id
+LEFT JOIN FileAgg       fa ON s.study_id = fa.study_id
+LEFT JOIN Publications  pub ON s.study_id = pub.study_id
+LEFT JOIN Personnel     pr  ON s.study_id = pr.study_id
+LEFT JOIN Funding       fd  ON s.study_id = fd.study_id;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    COALESCE(smp.sample_id, smp.id)                           AS "Sample ID",
+    COALESCE(prt.participant_id, prt.id)                      AS "Participant ID",
+    std.dbgap_accession                                       AS "Study ID",
+    COALESCE(smp.anatomic_site, '')                           AS "Sample Anatomic Site",
+    COALESCE(
+        CASE
+            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported'
+            ELSE CAST(smp.participant_age_at_collection AS TEXT)
+        END,
+        '0'
+    )                                                         AS "Age at Sample Collection (days)",
+    COALESCE(smp.sample_tumor_status, '')                     AS "Sample Tumor Status",
+    COALESCE(smp.tumor_classification, '')                    AS "Sample Tumor Classification",
+    CASE
+        WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis
+        ELSE NULL
+    END                                                       AS "Sample Diagnosis",
+    COALESCE(
+        CASE
+            WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis_category
+            ELSE NULL
+        END, ''
+    )                                                         AS "Diagnosis_Category"
+FROM df_study std
+JOIN df_consent_group  cg  ON std.id = cg."study.id"
+JOIN df_participant    prt ON cg.id  = prt."consent_group.id"
+LEFT JOIN df_sample    smp ON prt.id = smp."participant.id"
+LEFT JOIN df_diagnosis dgn ON prt.id = dgn."participant.id"
+WHERE std.dbgap_accession = 'phs000463'
+  AND prt.sex_at_birth = 'Male'
+  AND EXISTS (
+        SELECT 1
+        FROM df_diagnosis d
+        WHERE d."participant.id" = prt.id
+          AND d.diagnosis = 'Acute Lymphoblastic Leukemia, NOS'
+  )
+ORDER BY COALESCE(smp.sample_id, smp.id) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH file_data AS (
+  SELECT
+    cmf.file_name,
+    REPLACE(COALESCE(cmf.data_category, ''), ';', ', ') AS data_category,
+    COALESCE(cmf.file_description, '')                  AS file_description,
+    cmf.file_type,
+    cmf.file_access,
+    cmf.file_size,
+    cmf."study.id"        AS study_row_id,
+    cmf."participant.id"  AS participant_row_id
+  FROM df_clinical_measure_file cmf
+)
 SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' AND prt.sex_at_birth = 'Male' and dgn.diagnosis = 'Acute Lymphoblastic Leukemia, NOS'
-ORDER BY 
-    prt.participant_id ASC limit 100;</t>
-  </si>
-  <si>
-    <t>WITH Study AS (
-    SELECT DISTINCT 
-        std.study_name AS "Study_Name",
-        std.dbgap_accession AS "Study_ID",
-        std.study_status AS "Study_Status"
-    FROM df_study std 
-    WHERE std.dbgap_accession = 'phs000463'
-),
-diagnosis AS (
-    SELECT study_id, 
-        GROUP_CONCAT(diagcounts, ' ') AS diagcount 
-    FROM (
-        SELECT 'phs000463' AS study_id,  
-            diagnosis || ' (' || d_count || ')' AS diagcounts  -- Added space before '('
-        FROM (
-            SELECT ROW_NUMBER() OVER() AS row_num, 
-                dgn.diagnosis AS diagnosis,
-                COUNT(*) AS d_count 
-            FROM df_diagnosis dgn 
-            GROUP BY dgn.diagnosis 
-            ORDER BY d_count DESC
-        ) 
-        WHERE row_num &lt;= 5
-    )
-),
-diagnosisas AS (
-    SELECT study_id, 
-        GROUP_CONCAT(anatcounts, ' ') AS anatcount 
-    FROM (
-        SELECT 'phs000463' AS study_id,  
-            anat || ' (' || as_count || ')' AS anatcounts  -- Added space before '('
-        FROM (
-            SELECT ROW_NUMBER() OVER() AS row_num, 
-                dgn1.anatomic_site AS anat, 
-                COUNT(*) AS as_count 
-            FROM df_diagnosis dgn1 
-            GROUP BY dgn1.anatomic_site 
-            ORDER BY as_count DESC
-        ) 
-        WHERE row_num &lt;= 5
-    )
-),
-participants AS (
-    SELECT 'phs000463' AS study_id, 
-        COUNT(*) AS p_count 
-    FROM df_participant prt 
-),
-sample AS (
-    SELECT 'phs000463' AS study_id, 
-        COUNT(DISTINCT sample_id) AS s_count 
-    FROM df_sample
-),
-total_files AS (
-    SELECT 'phs000463' AS study_id, 
-        COUNT(*) AS file_count 
-    FROM df_clinical_measure_file
-),
-files AS (
-    SELECT study_id, 
-        GROUP_CONCAT(filecounts, ' ') AS file 
-    FROM (
-        SELECT 'phs000463' AS study_id,  
-            file_type || ' (' || filecount || ')' AS filecounts 
-        FROM (
-            SELECT ROW_NUMBER() OVER() AS row_num, 
-                file_type, 
-                COUNT(*) AS filecount 
-            FROM df_clinical_measure_file
-            GROUP BY file_type 
-            ORDER BY filecount DESC
-        ) 
-        WHERE row_num &lt;= 5
-    )
-),
-publications AS (
-    SELECT 'phs000463' AS study_id, 
-        GROUP_CONCAT(pubmed_id, ';') AS pubmeds 
-    FROM df_publication
-),
-personnel AS (
-    SELECT 'phs000463' AS study_id, 
-        GROUP_CONCAT(personnel_name, ';') AS name 
-    FROM df_study_personnel
-),
-funding AS (
-    SELECT 'phs000463' AS study_id, 
-        GROUP_CONCAT(grant_id, ';') AS grant 
-    FROM (
-        SELECT DISTINCT grant_id FROM df_study_funding
-    )
-)
-SELECT 
-    s.study_name AS "Study Name",
-    s.study_id AS "Study ID",
-    s.study_status AS "Study Status",
-    d.diagcount AS "Diagnosis (Top 5)",
-    da.anatcount AS "Diagnosis Anatomic Site (Top 5)",
-    p.p_count AS "Number of Participants",
-    smp.s_count AS "Number of Samples",
-    tf.file_count AS "Number of Files",
-    f.file AS "File Type (Top 5)",
-    pub.pubmeds AS "PubMed ID",
-    pr.name AS "Principal Investigator(s)",
-    fd.grant AS "Grant ID"
-FROM Study s
-LEFT JOIN diagnosis d ON s.study_id = d.study_id
-LEFT JOIN diagnosisas da ON s.study_id = da.study_id
-LEFT JOIN participants p ON s.study_id = p.study_id
-LEFT JOIN sample smp ON s.study_id = smp.study_id
-LEFT JOIN total_files tf ON s.study_id = tf.study_id
-LEFT JOIN files f ON s.study_id = f.study_id
-LEFT JOIN publications pub ON s.study_id = pub.study_id
-LEFT JOIN personnel pr ON s.study_id = pr.study_id
-LEFT JOIN funding fd ON s.study_id = fd.study_id;  -- Changed alias from 'f' to 'fd' here</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    COALESCE(
-        CASE 
-            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' 
-            ELSE smp.participant_age_at_collection 
-        END, 
-        0
-    ) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON smp.id = dgn."sample.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' 
-    AND prt.sex_at_birth = 'Male' 
-    AND dgn.diagnosis = 'Acute Lymphoblastic Leukemia, NOS' 
-    AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC;</t>
+  fd.file_name                               AS "File Name",
+  fd.data_category                           AS "Data Category",
+  fd.file_description                        AS "File Description",
+  fd.file_type                               AS "File Type",
+  CASE
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2)
+             = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2)
+             = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / 1024.0, 2)
+             = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+        ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
+      END
+    ELSE
+      CASE
+        WHEN ROUND(COALESCE(fd.file_size, 0), 2)
+             = CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT)
+        THEN CAST(CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT) AS TEXT) || ' Bytes'
+        ELSE ROUND(COALESCE(fd.file_size, 0), 2) || ' Bytes'
+      END
+  END                                         AS "File Size",
+  fd.file_access                              AS "File Access",
+  std.dbgap_accession                         AS "Study ID",
+  COALESCE(prt.participant_id, '')            AS "Participant ID",
+  ''                                          AS "Sample ID"   -- clinical files aren't sample-level here
+FROM df_study std
+JOIN file_data fd
+  ON std.id = fd.study_row_id
+LEFT JOIN df_participant prt
+  ON prt.id = fd.participant_row_id
+WHERE std.dbgap_accession = 'phs000463'
+ORDER BY fd.file_name
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -712,19 +755,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="47.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -741,12 +784,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="355.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="355" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>12</v>
@@ -758,37 +801,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>